<commit_message>
Best time to buy and sell stocks 2
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="321">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1664,7 +1664,9 @@
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">

</xml_diff>

<commit_message>
all duplicates in string
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/largest-rectangle-in-histogram/</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Strings</t>
@@ -1174,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1198,6 +1201,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -1541,9 +1547,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="136.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="136.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1867,8 +1873,8 @@
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>34</v>
+      <c r="B32" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C32" s="6"/>
     </row>
@@ -1880,7 +1886,7 @@
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="4"/>
       <c r="B34" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C34" s="8"/>
     </row>
@@ -1889,16 +1895,18 @@
         <v>9</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C36" s="6"/>
     </row>
@@ -1907,7 +1915,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C37" s="6"/>
     </row>
@@ -1916,7 +1924,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C38" s="6"/>
     </row>
@@ -1925,7 +1933,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C39" s="6"/>
     </row>
@@ -1934,7 +1942,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C40" s="6"/>
     </row>
@@ -1943,7 +1951,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C41" s="6"/>
     </row>
@@ -1952,7 +1960,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C42" s="6"/>
     </row>
@@ -1961,7 +1969,7 @@
         <v>5</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C43" s="6"/>
     </row>
@@ -1970,7 +1978,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C44" s="6"/>
     </row>
@@ -1979,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C45" s="6"/>
     </row>
@@ -1988,7 +1996,7 @@
         <v>5</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C46" s="6"/>
     </row>
@@ -1997,7 +2005,7 @@
         <v>5</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C47" s="6"/>
     </row>
@@ -2006,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C48" s="6"/>
     </row>
@@ -2015,7 +2023,7 @@
         <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C49" s="6"/>
     </row>
@@ -2024,7 +2032,7 @@
         <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C50" s="6"/>
     </row>
@@ -2033,7 +2041,7 @@
         <v>33</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C51" s="6"/>
     </row>
@@ -2042,7 +2050,7 @@
         <v>33</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C52" s="6"/>
     </row>
@@ -2051,7 +2059,7 @@
         <v>33</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C53" s="6"/>
     </row>
@@ -2060,7 +2068,7 @@
         <v>33</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C54" s="6"/>
     </row>
@@ -2072,7 +2080,7 @@
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="4"/>
       <c r="B56" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C56" s="8"/>
     </row>
@@ -2081,7 +2089,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C57" s="6"/>
     </row>
@@ -2090,7 +2098,7 @@
         <v>5</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C58" s="6"/>
     </row>
@@ -2099,7 +2107,7 @@
         <v>5</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C59" s="6"/>
     </row>
@@ -2117,7 +2125,7 @@
         <v>5</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C61" s="6"/>
     </row>
@@ -2129,7 +2137,7 @@
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="4"/>
       <c r="B63" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C63" s="8"/>
     </row>
@@ -2138,7 +2146,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C64" s="6"/>
     </row>
@@ -2147,7 +2155,7 @@
         <v>9</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C65" s="6"/>
     </row>
@@ -2156,7 +2164,7 @@
         <v>9</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C66" s="6"/>
     </row>
@@ -2165,7 +2173,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C67" s="6"/>
     </row>
@@ -2174,7 +2182,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C68" s="6"/>
     </row>
@@ -2183,7 +2191,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C69" s="6"/>
     </row>
@@ -2192,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C70" s="6"/>
     </row>
@@ -2201,7 +2209,7 @@
         <v>9</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C71" s="6"/>
     </row>
@@ -2210,7 +2218,7 @@
         <v>9</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C72" s="6"/>
     </row>
@@ -2219,7 +2227,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C73" s="6"/>
     </row>
@@ -2228,7 +2236,7 @@
         <v>5</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C74" s="6"/>
     </row>
@@ -2237,7 +2245,7 @@
         <v>5</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C75" s="6"/>
     </row>
@@ -2249,7 +2257,7 @@
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="4"/>
       <c r="B77" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C77" s="8"/>
     </row>
@@ -2258,7 +2266,7 @@
         <v>9</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C78" s="6"/>
     </row>
@@ -2267,7 +2275,7 @@
         <v>9</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C79" s="6"/>
     </row>
@@ -2276,7 +2284,7 @@
         <v>9</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C80" s="6"/>
     </row>
@@ -2285,7 +2293,7 @@
         <v>9</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C81" s="6"/>
     </row>
@@ -2294,7 +2302,7 @@
         <v>5</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C82" s="6"/>
     </row>
@@ -2302,17 +2310,17 @@
       <c r="A83" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" s="10"/>
+      <c r="B83" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C83" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C84" s="6"/>
     </row>
@@ -2320,26 +2328,26 @@
       <c r="A85" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C85" s="10"/>
+      <c r="B85" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C86" s="10"/>
+      <c r="B86" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C87" s="6"/>
     </row>
@@ -2348,7 +2356,7 @@
         <v>33</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C88" s="6"/>
     </row>
@@ -2357,7 +2365,7 @@
         <v>33</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C89" s="6"/>
     </row>
@@ -2365,28 +2373,28 @@
       <c r="A90" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B90" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C90" s="10"/>
+      <c r="B90" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B91" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C91" s="10"/>
+      <c r="B91" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B92" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C92" s="10"/>
+      <c r="B92" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="4"/>
@@ -2400,17 +2408,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="4"/>
-      <c r="B95" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C95" s="12"/>
+      <c r="B95" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C96" s="6"/>
     </row>
@@ -2419,7 +2427,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C97" s="6"/>
     </row>
@@ -2428,7 +2436,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C98" s="6"/>
     </row>
@@ -2437,7 +2445,7 @@
         <v>9</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C99" s="6"/>
     </row>
@@ -2446,7 +2454,7 @@
         <v>9</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C100" s="6"/>
     </row>
@@ -2455,7 +2463,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C101" s="6"/>
     </row>
@@ -2464,7 +2472,7 @@
         <v>9</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C102" s="6"/>
     </row>
@@ -2473,7 +2481,7 @@
         <v>9</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C103" s="6"/>
     </row>
@@ -2482,7 +2490,7 @@
         <v>9</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C104" s="6"/>
     </row>
@@ -2491,7 +2499,7 @@
         <v>9</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C105" s="6"/>
     </row>
@@ -2500,7 +2508,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C106" s="6"/>
     </row>
@@ -2509,7 +2517,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C107" s="6"/>
     </row>
@@ -2518,7 +2526,7 @@
         <v>5</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C108" s="6"/>
     </row>
@@ -2527,7 +2535,7 @@
         <v>5</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C109" s="6"/>
     </row>
@@ -2536,7 +2544,7 @@
         <v>5</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C110" s="6"/>
     </row>
@@ -2545,7 +2553,7 @@
         <v>5</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C111" s="6"/>
     </row>
@@ -2554,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C112" s="6"/>
     </row>
@@ -2563,7 +2571,7 @@
         <v>5</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C113" s="6"/>
     </row>
@@ -2572,7 +2580,7 @@
         <v>5</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C114" s="6"/>
     </row>
@@ -2581,7 +2589,7 @@
         <v>5</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C115" s="6"/>
     </row>
@@ -2590,7 +2598,7 @@
         <v>5</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C116" s="6"/>
     </row>
@@ -2599,7 +2607,7 @@
         <v>5</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C117" s="6"/>
     </row>
@@ -2608,7 +2616,7 @@
         <v>5</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C118" s="6"/>
     </row>
@@ -2617,7 +2625,7 @@
         <v>5</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C119" s="6"/>
     </row>
@@ -2626,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C120" s="6"/>
     </row>
@@ -2635,7 +2643,7 @@
         <v>33</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C121" s="6"/>
     </row>
@@ -2644,7 +2652,7 @@
         <v>33</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C122" s="6"/>
     </row>
@@ -2653,7 +2661,7 @@
         <v>33</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C123" s="6"/>
     </row>
@@ -2662,7 +2670,7 @@
         <v>33</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C124" s="6"/>
     </row>
@@ -2671,7 +2679,7 @@
         <v>33</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C125" s="6"/>
     </row>
@@ -2682,10 +2690,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="4"/>
-      <c r="B127" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C127" s="12"/>
+      <c r="B127" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C127" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="4"/>
@@ -2697,7 +2705,7 @@
         <v>9</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C129" s="6"/>
     </row>
@@ -2706,7 +2714,7 @@
         <v>9</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C130" s="6"/>
     </row>
@@ -2715,7 +2723,7 @@
         <v>9</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C131" s="6"/>
     </row>
@@ -2724,7 +2732,7 @@
         <v>9</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C132" s="6"/>
     </row>
@@ -2733,7 +2741,7 @@
         <v>9</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C133" s="6"/>
     </row>
@@ -2742,7 +2750,7 @@
         <v>9</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C134" s="6"/>
     </row>
@@ -2751,7 +2759,7 @@
         <v>9</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C135" s="6"/>
     </row>
@@ -2760,7 +2768,7 @@
         <v>5</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C136" s="6"/>
     </row>
@@ -2769,7 +2777,7 @@
         <v>5</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C137" s="6"/>
     </row>
@@ -2778,7 +2786,7 @@
         <v>5</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C138" s="6"/>
     </row>
@@ -2787,7 +2795,7 @@
         <v>5</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C139" s="6"/>
     </row>
@@ -2796,7 +2804,7 @@
         <v>5</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C140" s="6"/>
     </row>
@@ -2805,7 +2813,7 @@
         <v>5</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C141" s="6"/>
     </row>
@@ -2814,7 +2822,7 @@
         <v>5</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C142" s="6"/>
     </row>
@@ -2823,7 +2831,7 @@
         <v>5</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C143" s="6"/>
     </row>
@@ -2832,7 +2840,7 @@
         <v>5</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C144" s="6"/>
     </row>
@@ -2841,7 +2849,7 @@
         <v>5</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C145" s="6"/>
     </row>
@@ -2850,7 +2858,7 @@
         <v>33</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C146" s="6"/>
     </row>
@@ -2859,7 +2867,7 @@
         <v>33</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C147" s="6"/>
     </row>
@@ -2868,7 +2876,7 @@
         <v>33</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C148" s="6"/>
     </row>
@@ -2884,17 +2892,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="4"/>
-      <c r="B151" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C151" s="14"/>
+      <c r="B151" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C151" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C152" s="6"/>
     </row>
@@ -2903,7 +2911,7 @@
         <v>9</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C153" s="6"/>
     </row>
@@ -2912,7 +2920,7 @@
         <v>9</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C154" s="6"/>
     </row>
@@ -2921,7 +2929,7 @@
         <v>9</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C155" s="6"/>
     </row>
@@ -2930,7 +2938,7 @@
         <v>9</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C156" s="6"/>
     </row>
@@ -2939,7 +2947,7 @@
         <v>9</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C157" s="6"/>
     </row>
@@ -2948,7 +2956,7 @@
         <v>9</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C158" s="6"/>
     </row>
@@ -2957,7 +2965,7 @@
         <v>9</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C159" s="6"/>
     </row>
@@ -2966,7 +2974,7 @@
         <v>9</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C160" s="6"/>
     </row>
@@ -2975,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C161" s="6"/>
     </row>
@@ -2984,7 +2992,7 @@
         <v>9</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C162" s="6"/>
     </row>
@@ -2993,7 +3001,7 @@
         <v>9</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C163" s="6"/>
     </row>
@@ -3002,7 +3010,7 @@
         <v>9</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C164" s="6"/>
     </row>
@@ -3011,7 +3019,7 @@
         <v>9</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C165" s="6"/>
     </row>
@@ -3020,7 +3028,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C166" s="6"/>
     </row>
@@ -3029,7 +3037,7 @@
         <v>9</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C167" s="6"/>
     </row>
@@ -3038,7 +3046,7 @@
         <v>9</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C168" s="6"/>
     </row>
@@ -3047,7 +3055,7 @@
         <v>9</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C169" s="6"/>
     </row>
@@ -3056,7 +3064,7 @@
         <v>5</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C170" s="6"/>
     </row>
@@ -3065,7 +3073,7 @@
         <v>5</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C171" s="6"/>
     </row>
@@ -3074,7 +3082,7 @@
         <v>5</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C172" s="6"/>
     </row>
@@ -3083,7 +3091,7 @@
         <v>5</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C173" s="6"/>
     </row>
@@ -3092,7 +3100,7 @@
         <v>5</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C174" s="6"/>
     </row>
@@ -3101,7 +3109,7 @@
         <v>5</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C175" s="6"/>
     </row>
@@ -3110,7 +3118,7 @@
         <v>5</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C176" s="6"/>
     </row>
@@ -3119,7 +3127,7 @@
         <v>5</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C177" s="6"/>
     </row>
@@ -3128,7 +3136,7 @@
         <v>5</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C178" s="6"/>
     </row>
@@ -3137,7 +3145,7 @@
         <v>5</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C179" s="6"/>
     </row>
@@ -3146,7 +3154,7 @@
         <v>5</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C180" s="6"/>
     </row>
@@ -3155,7 +3163,7 @@
         <v>5</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C181" s="6"/>
     </row>
@@ -3164,7 +3172,7 @@
         <v>5</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C182" s="6"/>
     </row>
@@ -3173,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C183" s="6"/>
     </row>
@@ -3182,7 +3190,7 @@
         <v>5</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C184" s="6"/>
     </row>
@@ -3191,7 +3199,7 @@
         <v>5</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C185" s="6"/>
     </row>
@@ -3200,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C186" s="6"/>
     </row>
@@ -3209,7 +3217,7 @@
         <v>5</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C187" s="6"/>
     </row>
@@ -3218,7 +3226,7 @@
         <v>5</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C188" s="6"/>
     </row>
@@ -3227,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C189" s="6"/>
     </row>
@@ -3236,7 +3244,7 @@
         <v>33</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C190" s="6"/>
     </row>
@@ -3245,7 +3253,7 @@
         <v>33</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C191" s="6"/>
     </row>
@@ -3254,7 +3262,7 @@
         <v>33</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C192" s="6"/>
     </row>
@@ -3263,7 +3271,7 @@
         <v>33</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C193" s="6"/>
     </row>
@@ -3272,7 +3280,7 @@
         <v>33</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C194" s="6"/>
     </row>
@@ -3281,7 +3289,7 @@
         <v>33</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C195" s="6"/>
     </row>
@@ -3290,7 +3298,7 @@
         <v>33</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C196" s="6"/>
     </row>
@@ -3299,7 +3307,7 @@
         <v>33</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C197" s="6"/>
     </row>
@@ -3308,7 +3316,7 @@
         <v>33</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C198" s="6"/>
     </row>
@@ -3317,7 +3325,7 @@
         <v>33</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C199" s="6"/>
     </row>
@@ -3329,7 +3337,7 @@
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
       <c r="A201" s="4"/>
       <c r="B201" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C201" s="8"/>
     </row>
@@ -3338,7 +3346,7 @@
         <v>9</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C202" s="6"/>
     </row>
@@ -3347,7 +3355,7 @@
         <v>9</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C203" s="6"/>
     </row>
@@ -3356,7 +3364,7 @@
         <v>9</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C204" s="6"/>
     </row>
@@ -3365,7 +3373,7 @@
         <v>9</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C205" s="6"/>
     </row>
@@ -3374,7 +3382,7 @@
         <v>9</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C206" s="6"/>
     </row>
@@ -3383,7 +3391,7 @@
         <v>9</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C207" s="6"/>
     </row>
@@ -3392,7 +3400,7 @@
         <v>9</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C208" s="6"/>
     </row>
@@ -3401,7 +3409,7 @@
         <v>5</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C209" s="6"/>
     </row>
@@ -3410,7 +3418,7 @@
         <v>5</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C210" s="6"/>
     </row>
@@ -3419,7 +3427,7 @@
         <v>5</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C211" s="6"/>
     </row>
@@ -3428,7 +3436,7 @@
         <v>5</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C212" s="6"/>
     </row>
@@ -3437,7 +3445,7 @@
         <v>5</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C213" s="6"/>
     </row>
@@ -3446,7 +3454,7 @@
         <v>5</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C214" s="6"/>
     </row>
@@ -3455,7 +3463,7 @@
         <v>5</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C215" s="6"/>
     </row>
@@ -3464,7 +3472,7 @@
         <v>5</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C216" s="6"/>
     </row>
@@ -3473,7 +3481,7 @@
         <v>5</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C217" s="6"/>
     </row>
@@ -3482,7 +3490,7 @@
         <v>5</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C218" s="6"/>
     </row>
@@ -3491,7 +3499,7 @@
         <v>5</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C219" s="6"/>
     </row>
@@ -3500,7 +3508,7 @@
         <v>5</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C220" s="6"/>
     </row>
@@ -3509,7 +3517,7 @@
         <v>5</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C221" s="6"/>
     </row>
@@ -3518,7 +3526,7 @@
         <v>5</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C222" s="6"/>
     </row>
@@ -3527,7 +3535,7 @@
         <v>5</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C223" s="6"/>
     </row>
@@ -3536,7 +3544,7 @@
         <v>5</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C224" s="6"/>
     </row>
@@ -3545,7 +3553,7 @@
         <v>5</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C225" s="6"/>
     </row>
@@ -3554,7 +3562,7 @@
         <v>5</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C226" s="6"/>
     </row>
@@ -3563,7 +3571,7 @@
         <v>5</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C227" s="6"/>
     </row>
@@ -3572,7 +3580,7 @@
         <v>5</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C228" s="6"/>
     </row>
@@ -3581,7 +3589,7 @@
         <v>33</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C229" s="6"/>
     </row>
@@ -3590,7 +3598,7 @@
         <v>33</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C230" s="6"/>
     </row>
@@ -3599,7 +3607,7 @@
         <v>33</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C231" s="6"/>
     </row>
@@ -3608,7 +3616,7 @@
         <v>33</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C232" s="6"/>
     </row>
@@ -3617,7 +3625,7 @@
         <v>33</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C233" s="6"/>
     </row>
@@ -3626,7 +3634,7 @@
         <v>33</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C234" s="6"/>
     </row>
@@ -3635,7 +3643,7 @@
         <v>33</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C235" s="6"/>
     </row>
@@ -3644,7 +3652,7 @@
         <v>33</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C236" s="6"/>
     </row>
@@ -3653,7 +3661,7 @@
         <v>33</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C237" s="6"/>
     </row>
@@ -3662,7 +3670,7 @@
         <v>33</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C238" s="6"/>
     </row>
@@ -3674,7 +3682,7 @@
     <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="18.75">
       <c r="A240" s="4"/>
       <c r="B240" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C240" s="8"/>
     </row>
@@ -3683,7 +3691,7 @@
         <v>5</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C241" s="6"/>
     </row>
@@ -3692,7 +3700,7 @@
         <v>5</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C242" s="6"/>
     </row>
@@ -3701,7 +3709,7 @@
         <v>5</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C243" s="6"/>
     </row>
@@ -3710,7 +3718,7 @@
         <v>5</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C244" s="6"/>
     </row>
@@ -3719,7 +3727,7 @@
         <v>33</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C245" s="6"/>
     </row>
@@ -3728,7 +3736,7 @@
         <v>33</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C246" s="6"/>
     </row>
@@ -3739,10 +3747,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75">
       <c r="A248" s="4"/>
-      <c r="B248" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C248" s="12"/>
+      <c r="B248" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C248" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75">
       <c r="A249" s="4"/>
@@ -3751,91 +3759,91 @@
     </row>
     <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="18.75">
       <c r="A250" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C250" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="18.75">
       <c r="A251" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C251" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="18.75">
       <c r="A252" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C252" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18.75">
       <c r="A253" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C253" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="18.75">
       <c r="A254" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C254" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="18.75">
       <c r="A255" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C255" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="18.75">
       <c r="A256" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C256" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="18.75">
       <c r="A257" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C257" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75">
       <c r="A258" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C258" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75">
       <c r="A259" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C259" s="6"/>
     </row>
@@ -3844,7 +3852,7 @@
         <v>33</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C260" s="6"/>
     </row>
@@ -3853,7 +3861,7 @@
         <v>33</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C261" s="6"/>
     </row>
@@ -3862,7 +3870,7 @@
         <v>33</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C262" s="6"/>
     </row>
@@ -3871,7 +3879,7 @@
         <v>33</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C263" s="6"/>
     </row>
@@ -3883,7 +3891,7 @@
     <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="18.75">
       <c r="A265" s="4"/>
       <c r="B265" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C265" s="8"/>
     </row>
@@ -3892,7 +3900,7 @@
         <v>9</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C266" s="6"/>
     </row>
@@ -3901,7 +3909,7 @@
         <v>9</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C267" s="6"/>
     </row>
@@ -3910,7 +3918,7 @@
         <v>9</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C268" s="6"/>
     </row>
@@ -3919,7 +3927,7 @@
         <v>9</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C269" s="6"/>
     </row>
@@ -3928,7 +3936,7 @@
         <v>5</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C270" s="6"/>
     </row>
@@ -3937,7 +3945,7 @@
         <v>5</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C271" s="6"/>
     </row>
@@ -3946,7 +3954,7 @@
         <v>5</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C272" s="6"/>
     </row>
@@ -3955,7 +3963,7 @@
         <v>5</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C273" s="6"/>
     </row>
@@ -3964,7 +3972,7 @@
         <v>5</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C274" s="6"/>
     </row>
@@ -3973,7 +3981,7 @@
         <v>5</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C275" s="6"/>
     </row>
@@ -3982,7 +3990,7 @@
         <v>5</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C276" s="6"/>
     </row>
@@ -3991,7 +3999,7 @@
         <v>5</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C277" s="6"/>
     </row>
@@ -4000,7 +4008,7 @@
         <v>5</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C278" s="6"/>
     </row>
@@ -4009,7 +4017,7 @@
         <v>5</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C279" s="6"/>
     </row>
@@ -4018,7 +4026,7 @@
         <v>5</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C280" s="6"/>
     </row>
@@ -4027,7 +4035,7 @@
         <v>5</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C281" s="6"/>
     </row>
@@ -4036,7 +4044,7 @@
         <v>5</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C282" s="6"/>
     </row>
@@ -4045,7 +4053,7 @@
         <v>5</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C283" s="6"/>
     </row>
@@ -4054,7 +4062,7 @@
         <v>5</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C284" s="6"/>
     </row>
@@ -4063,7 +4071,7 @@
         <v>33</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C285" s="6"/>
     </row>
@@ -4072,7 +4080,7 @@
         <v>33</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C286" s="6"/>
     </row>
@@ -4081,7 +4089,7 @@
         <v>33</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C287" s="6"/>
     </row>
@@ -4090,7 +4098,7 @@
         <v>33</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C288" s="6"/>
     </row>
@@ -4099,7 +4107,7 @@
         <v>33</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C289" s="6"/>
     </row>
@@ -4108,7 +4116,7 @@
         <v>33</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C290" s="6"/>
     </row>
@@ -4117,7 +4125,7 @@
         <v>33</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C291" s="6"/>
     </row>
@@ -4126,7 +4134,7 @@
         <v>33</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C292" s="6"/>
     </row>
@@ -4135,7 +4143,7 @@
         <v>33</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C293" s="6"/>
     </row>
@@ -4144,7 +4152,7 @@
         <v>33</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C294" s="6"/>
     </row>
@@ -4153,7 +4161,7 @@
         <v>33</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C295" s="6"/>
     </row>
@@ -4165,7 +4173,7 @@
     <row x14ac:dyDescent="0.25" r="297" customHeight="1" ht="18.75">
       <c r="A297" s="4"/>
       <c r="B297" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C297" s="8"/>
     </row>
@@ -4183,7 +4191,7 @@
         <v>5</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C299" s="6"/>
     </row>
@@ -4192,7 +4200,7 @@
         <v>5</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C300" s="6"/>
     </row>
@@ -4209,97 +4217,97 @@
     <row x14ac:dyDescent="0.25" r="303" customHeight="1" ht="18.75">
       <c r="A303" s="4"/>
       <c r="B303" s="7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C303" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="304" customHeight="1" ht="18.75">
       <c r="A304" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C304" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="305" customHeight="1" ht="18.75">
       <c r="A305" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C305" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="306" customHeight="1" ht="18.75">
       <c r="A306" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C306" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="307" customHeight="1" ht="18.75">
       <c r="A307" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C307" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="308" customHeight="1" ht="18.75">
       <c r="A308" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C308" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="309" customHeight="1" ht="18.75">
       <c r="A309" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C309" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="310" customHeight="1" ht="18.75">
       <c r="A310" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C310" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="311" customHeight="1" ht="18.75">
       <c r="A311" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C311" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="312" customHeight="1" ht="18.75">
       <c r="A312" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C312" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="313" customHeight="1" ht="18.75">
       <c r="A313" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C313" s="6"/>
     </row>
@@ -4315,17 +4323,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="316" customHeight="1" ht="18.75">
       <c r="A316" s="4"/>
-      <c r="B316" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="C316" s="12"/>
+      <c r="B316" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C316" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="317" customHeight="1" ht="18.75">
       <c r="A317" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C317" s="6"/>
     </row>
@@ -4334,7 +4342,7 @@
         <v>5</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C318" s="6"/>
     </row>
@@ -4343,7 +4351,7 @@
         <v>5</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C319" s="6"/>
     </row>
@@ -4352,7 +4360,7 @@
         <v>5</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C320" s="6"/>
     </row>
@@ -4361,7 +4369,7 @@
         <v>5</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C321" s="6"/>
     </row>
@@ -4370,7 +4378,7 @@
         <v>5</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C322" s="6"/>
     </row>
@@ -4379,7 +4387,7 @@
         <v>5</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C323" s="6"/>
     </row>
@@ -4388,7 +4396,7 @@
         <v>5</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C324" s="6"/>
     </row>
@@ -4397,7 +4405,7 @@
         <v>33</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C325" s="6"/>
     </row>
@@ -4406,7 +4414,7 @@
         <v>33</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C326" s="6"/>
     </row>
@@ -4415,7 +4423,7 @@
         <v>33</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C327" s="6"/>
     </row>
@@ -4424,7 +4432,7 @@
         <v>33</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C328" s="6"/>
     </row>
@@ -4433,7 +4441,7 @@
         <v>33</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C329" s="6"/>
     </row>
@@ -4442,7 +4450,7 @@
         <v>33</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C330" s="6"/>
     </row>
@@ -4451,7 +4459,7 @@
         <v>33</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C331" s="6"/>
     </row>
@@ -4460,7 +4468,7 @@
         <v>33</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C332" s="6"/>
     </row>
@@ -4469,7 +4477,7 @@
         <v>33</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C333" s="6"/>
     </row>
@@ -4478,7 +4486,7 @@
         <v>33</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C334" s="6"/>
     </row>
@@ -4489,44 +4497,44 @@
     </row>
     <row x14ac:dyDescent="0.25" r="336" customHeight="1" ht="18.75">
       <c r="A336" s="4"/>
-      <c r="B336" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="C336" s="16"/>
+      <c r="B336" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="C336" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="337" customHeight="1" ht="18.75">
       <c r="A337" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C337" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="338" customHeight="1" ht="18.75">
       <c r="A338" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C338" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="339" customHeight="1" ht="18.75">
       <c r="A339" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C339" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="340" customHeight="1" ht="18.75">
       <c r="A340" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C340" s="6"/>
     </row>
@@ -7826,8 +7834,8 @@
       <c r="C999" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1000" customHeight="1" ht="18.75">
-      <c r="A1000" s="17"/>
-      <c r="B1000" s="18"/>
+      <c r="A1000" s="18"/>
+      <c r="B1000" s="19"/>
       <c r="C1000" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Merge2dArrays class to merge two 2D arrays and calculate their combined length
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reverse-pairs/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-2d-arrays-by-summing-values/?envType=daily-question&amp;envId=2025-03-02</t>
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/print-all-possible-combinations-of-r-elements-in-a-given-array-of-size-n/</t>
@@ -1180,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1204,6 +1207,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
@@ -1544,15 +1550,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C1001"/>
+  <dimension ref="A1:C1002"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="20" width="98.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="21" width="98.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1822,13 +1828,15 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="4" t="s">
@@ -1837,70 +1845,68 @@
       <c r="B28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C28" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C29" s="6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="C32" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="4"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="4"/>
-      <c r="B34" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="B34" s="7"/>
       <c r="C34" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="4"/>
+      <c r="B35" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C35" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="4" t="s">
@@ -1948,7 +1954,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>43</v>
@@ -1986,7 +1992,9 @@
       <c r="B43" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="6"/>
+      <c r="C43" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="4" t="s">
@@ -1995,9 +2003,7 @@
       <c r="B44" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="4" t="s">
@@ -2006,7 +2012,9 @@
       <c r="B45" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="4" t="s">
@@ -2015,9 +2023,7 @@
       <c r="B46" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C46" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="4" t="s">
@@ -2026,7 +2032,9 @@
       <c r="B47" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="4" t="s">
@@ -2035,22 +2043,22 @@
       <c r="B48" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C48" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>53</v>
@@ -2059,7 +2067,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>54</v>
@@ -2068,7 +2076,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>55</v>
@@ -2077,7 +2085,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>56</v>
@@ -2086,7 +2094,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>57</v>
@@ -2094,25 +2102,25 @@
       <c r="C54" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="4"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="8"/>
+      <c r="A55" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="4"/>
-      <c r="B56" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="B56" s="7"/>
       <c r="C56" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="5" t="s">
+      <c r="A57" s="4"/>
+      <c r="B57" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="6"/>
+      <c r="C57" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="4" t="s">
@@ -2132,55 +2140,53 @@
       </c>
       <c r="C59" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+      <c r="A61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" s="6" t="s">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="4"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="4"/>
-      <c r="B64" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="B64" s="7"/>
       <c r="C64" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B65" s="5" t="s">
+      <c r="A65" s="4"/>
+      <c r="B65" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C65" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="4" t="s">
@@ -2200,7 +2206,9 @@
       <c r="B67" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="6"/>
+      <c r="C67" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="4" t="s">
@@ -2218,7 +2226,9 @@
       <c r="B69" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="6"/>
+      <c r="C69" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="4" t="s">
@@ -2258,7 +2268,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>73</v>
@@ -2284,25 +2294,25 @@
       <c r="C76" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="4"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="8"/>
+      <c r="A77" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="4"/>
-      <c r="B78" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="B78" s="7"/>
       <c r="C78" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="5" t="s">
+      <c r="A79" s="4"/>
+      <c r="B79" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="6"/>
+      <c r="C79" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="4" t="s">
@@ -2327,16 +2337,16 @@
         <v>9</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C82" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C83" s="6"/>
     </row>
@@ -2344,50 +2354,50 @@
       <c r="A84" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C84" s="11"/>
+      <c r="C84" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="6"/>
+      <c r="C85" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C86" s="11"/>
+      <c r="C86" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="11"/>
+      <c r="C87" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="6"/>
+      <c r="C88" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>86</v>
@@ -2396,7 +2406,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>87</v>
@@ -2405,35 +2415,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B91" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="11"/>
+      <c r="C91" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B92" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="11"/>
+      <c r="C92" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B93" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="11"/>
+      <c r="C93" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
-      <c r="A94" s="4"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="8"/>
+      <c r="A94" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C94" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="4"/>
@@ -2442,19 +2456,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="4"/>
-      <c r="B96" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C96" s="13"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97" s="5" t="s">
+      <c r="A97" s="4"/>
+      <c r="B97" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C97" s="6"/>
+      <c r="C97" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="4" t="s">
@@ -2557,7 +2567,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>104</v>
@@ -2674,7 +2684,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>117</v>
@@ -2683,7 +2693,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>118</v>
@@ -2692,7 +2702,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>119</v>
@@ -2701,7 +2711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>120</v>
@@ -2710,7 +2720,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>121</v>
@@ -2718,30 +2728,30 @@
       <c r="C126" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
-      <c r="A127" s="4"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="8"/>
+      <c r="A127" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C127" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="4"/>
-      <c r="B128" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C128" s="13"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="4"/>
-      <c r="B129" s="7"/>
-      <c r="C129" s="8"/>
+      <c r="B129" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C129" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
-      <c r="A130" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C130" s="6"/>
+      <c r="A130" s="4"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="4" t="s">
@@ -2799,7 +2809,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>130</v>
@@ -2889,7 +2899,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>140</v>
@@ -2898,7 +2908,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>141</v>
@@ -2907,7 +2917,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>142</v>
@@ -2915,9 +2925,13 @@
       <c r="C149" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
-      <c r="A150" s="4"/>
-      <c r="B150" s="7"/>
-      <c r="C150" s="8"/>
+      <c r="A150" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C150" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="4"/>
@@ -2926,19 +2940,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="4"/>
-      <c r="B152" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C152" s="15"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
-      <c r="A153" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B153" s="5" t="s">
+      <c r="A153" s="4"/>
+      <c r="B153" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C153" s="6"/>
+      <c r="C153" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="4" t="s">
@@ -3095,7 +3105,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>162</v>
@@ -3275,7 +3285,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B191" s="5" t="s">
         <v>182</v>
@@ -3284,7 +3294,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>183</v>
@@ -3293,7 +3303,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
       <c r="A193" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B193" s="5" t="s">
         <v>184</v>
@@ -3302,7 +3312,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
       <c r="A194" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B194" s="5" t="s">
         <v>185</v>
@@ -3311,7 +3321,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
       <c r="A195" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B195" s="5" t="s">
         <v>186</v>
@@ -3320,7 +3330,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
       <c r="A196" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B196" s="5" t="s">
         <v>187</v>
@@ -3329,7 +3339,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
       <c r="A197" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>188</v>
@@ -3338,7 +3348,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
       <c r="A198" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B198" s="5" t="s">
         <v>189</v>
@@ -3347,7 +3357,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
       <c r="A199" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B199" s="5" t="s">
         <v>190</v>
@@ -3356,7 +3366,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
       <c r="A200" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B200" s="5" t="s">
         <v>191</v>
@@ -3364,25 +3374,25 @@
       <c r="C200" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
-      <c r="A201" s="4"/>
-      <c r="B201" s="7"/>
-      <c r="C201" s="8"/>
+      <c r="A201" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C201" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
       <c r="A202" s="4"/>
-      <c r="B202" s="7" t="s">
-        <v>192</v>
-      </c>
+      <c r="B202" s="7"/>
       <c r="C202" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
-      <c r="A203" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B203" s="5" t="s">
+      <c r="A203" s="4"/>
+      <c r="B203" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C203" s="6"/>
+      <c r="C203" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75">
       <c r="A204" s="4" t="s">
@@ -3440,7 +3450,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75">
       <c r="A210" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B210" s="5" t="s">
         <v>200</v>
@@ -3620,7 +3630,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="18.75">
       <c r="A230" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B230" s="5" t="s">
         <v>220</v>
@@ -3629,7 +3639,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="18.75">
       <c r="A231" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B231" s="5" t="s">
         <v>221</v>
@@ -3638,7 +3648,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="18.75">
       <c r="A232" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B232" s="5" t="s">
         <v>222</v>
@@ -3647,7 +3657,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="18.75">
       <c r="A233" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B233" s="5" t="s">
         <v>223</v>
@@ -3656,7 +3666,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="18.75">
       <c r="A234" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B234" s="5" t="s">
         <v>224</v>
@@ -3665,7 +3675,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="18.75">
       <c r="A235" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B235" s="5" t="s">
         <v>225</v>
@@ -3674,7 +3684,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="18.75">
       <c r="A236" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B236" s="5" t="s">
         <v>226</v>
@@ -3683,7 +3693,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="18.75">
       <c r="A237" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B237" s="5" t="s">
         <v>227</v>
@@ -3692,7 +3702,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="18.75">
       <c r="A238" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B238" s="5" t="s">
         <v>228</v>
@@ -3701,7 +3711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="18.75">
       <c r="A239" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B239" s="5" t="s">
         <v>229</v>
@@ -3709,25 +3719,25 @@
       <c r="C239" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="18.75">
-      <c r="A240" s="4"/>
-      <c r="B240" s="7"/>
-      <c r="C240" s="8"/>
+      <c r="A240" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C240" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="18.75">
       <c r="A241" s="4"/>
-      <c r="B241" s="7" t="s">
-        <v>230</v>
-      </c>
+      <c r="B241" s="7"/>
       <c r="C241" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="18.75">
-      <c r="A242" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B242" s="5" t="s">
+      <c r="A242" s="4"/>
+      <c r="B242" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C242" s="6"/>
+      <c r="C242" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="18.75">
       <c r="A243" s="4" t="s">
@@ -3758,7 +3768,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="18.75">
       <c r="A246" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B246" s="5" t="s">
         <v>235</v>
@@ -3767,7 +3777,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="18.75">
       <c r="A247" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B247" s="5" t="s">
         <v>236</v>
@@ -3775,34 +3785,34 @@
       <c r="C247" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75">
-      <c r="A248" s="4"/>
-      <c r="B248" s="7"/>
-      <c r="C248" s="8"/>
+      <c r="A248" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C248" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="18.75">
       <c r="A249" s="4"/>
-      <c r="B249" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="C249" s="13"/>
+      <c r="B249" s="7"/>
+      <c r="C249" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="18.75">
       <c r="A250" s="4"/>
-      <c r="B250" s="7"/>
-      <c r="C250" s="8"/>
+      <c r="B250" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C250" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="18.75">
-      <c r="A251" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="B251" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C251" s="6"/>
+      <c r="A251" s="4"/>
+      <c r="B251" s="7"/>
+      <c r="C251" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="18.75">
       <c r="A252" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B252" s="5" t="s">
         <v>240</v>
@@ -3811,7 +3821,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18.75">
       <c r="A253" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B253" s="5" t="s">
         <v>241</v>
@@ -3820,7 +3830,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="18.75">
       <c r="A254" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B254" s="5" t="s">
         <v>242</v>
@@ -3829,7 +3839,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="18.75">
       <c r="A255" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B255" s="5" t="s">
         <v>243</v>
@@ -3838,7 +3848,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="18.75">
       <c r="A256" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B256" s="5" t="s">
         <v>244</v>
@@ -3847,7 +3857,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="18.75">
       <c r="A257" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B257" s="5" t="s">
         <v>245</v>
@@ -3856,7 +3866,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75">
       <c r="A258" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B258" s="5" t="s">
         <v>246</v>
@@ -3865,7 +3875,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75">
       <c r="A259" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B259" s="5" t="s">
         <v>247</v>
@@ -3874,7 +3884,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="18.75">
       <c r="A260" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B260" s="5" t="s">
         <v>248</v>
@@ -3883,7 +3893,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="18.75">
       <c r="A261" s="4" t="s">
-        <v>33</v>
+        <v>239</v>
       </c>
       <c r="B261" s="5" t="s">
         <v>249</v>
@@ -3892,7 +3902,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="18.75">
       <c r="A262" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B262" s="5" t="s">
         <v>250</v>
@@ -3901,7 +3911,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="18.75">
       <c r="A263" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>251</v>
@@ -3910,7 +3920,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="18.75">
       <c r="A264" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>252</v>
@@ -3918,25 +3928,25 @@
       <c r="C264" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="18.75">
-      <c r="A265" s="4"/>
-      <c r="B265" s="7"/>
-      <c r="C265" s="8"/>
+      <c r="A265" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C265" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="18.75">
       <c r="A266" s="4"/>
-      <c r="B266" s="7" t="s">
-        <v>253</v>
-      </c>
+      <c r="B266" s="7"/>
       <c r="C266" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="18.75">
-      <c r="A267" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B267" s="5" t="s">
+      <c r="A267" s="4"/>
+      <c r="B267" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C267" s="6"/>
+      <c r="C267" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="268" customHeight="1" ht="18.75">
       <c r="A268" s="4" t="s">
@@ -3967,7 +3977,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="18.75">
       <c r="A271" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B271" s="5" t="s">
         <v>258</v>
@@ -4102,7 +4112,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="286" customHeight="1" ht="18.75">
       <c r="A286" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B286" s="5" t="s">
         <v>273</v>
@@ -4111,7 +4121,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="287" customHeight="1" ht="18.75">
       <c r="A287" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B287" s="5" t="s">
         <v>274</v>
@@ -4120,7 +4130,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="288" customHeight="1" ht="18.75">
       <c r="A288" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>275</v>
@@ -4129,7 +4139,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="289" customHeight="1" ht="18.75">
       <c r="A289" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B289" s="5" t="s">
         <v>276</v>
@@ -4138,7 +4148,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="290" customHeight="1" ht="18.75">
       <c r="A290" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B290" s="5" t="s">
         <v>277</v>
@@ -4147,7 +4157,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="291" customHeight="1" ht="18.75">
       <c r="A291" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B291" s="5" t="s">
         <v>278</v>
@@ -4156,7 +4166,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="292" customHeight="1" ht="18.75">
       <c r="A292" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>279</v>
@@ -4165,7 +4175,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="293" customHeight="1" ht="18.75">
       <c r="A293" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B293" s="5" t="s">
         <v>280</v>
@@ -4174,7 +4184,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="294" customHeight="1" ht="18.75">
       <c r="A294" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B294" s="5" t="s">
         <v>281</v>
@@ -4183,7 +4193,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="295" customHeight="1" ht="18.75">
       <c r="A295" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B295" s="5" t="s">
         <v>282</v>
@@ -4192,7 +4202,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="296" customHeight="1" ht="18.75">
       <c r="A296" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>283</v>
@@ -4200,32 +4210,32 @@
       <c r="C296" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="297" customHeight="1" ht="18.75">
-      <c r="A297" s="4"/>
-      <c r="B297" s="7"/>
-      <c r="C297" s="8"/>
+      <c r="A297" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C297" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="298" customHeight="1" ht="18.75">
       <c r="A298" s="4"/>
-      <c r="B298" s="7" t="s">
-        <v>284</v>
-      </c>
+      <c r="B298" s="7"/>
       <c r="C298" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="299" customHeight="1" ht="18.75">
-      <c r="A299" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B299" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C299" s="6"/>
+      <c r="A299" s="4"/>
+      <c r="B299" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C299" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="300" customHeight="1" ht="18.75">
       <c r="A300" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>285</v>
+        <v>7</v>
       </c>
       <c r="C300" s="6"/>
     </row>
@@ -4239,9 +4249,13 @@
       <c r="C301" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="302" customHeight="1" ht="18.75">
-      <c r="A302" s="4"/>
-      <c r="B302" s="7"/>
-      <c r="C302" s="8"/>
+      <c r="A302" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C302" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="303" customHeight="1" ht="18.75">
       <c r="A303" s="4"/>
@@ -4250,23 +4264,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="304" customHeight="1" ht="18.75">
       <c r="A304" s="4"/>
-      <c r="B304" s="7" t="s">
-        <v>287</v>
-      </c>
+      <c r="B304" s="7"/>
       <c r="C304" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="305" customHeight="1" ht="18.75">
-      <c r="A305" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="B305" s="5" t="s">
+      <c r="A305" s="4"/>
+      <c r="B305" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C305" s="6"/>
+      <c r="C305" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="306" customHeight="1" ht="18.75">
       <c r="A306" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B306" s="5" t="s">
         <v>289</v>
@@ -4275,7 +4285,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="307" customHeight="1" ht="18.75">
       <c r="A307" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B307" s="5" t="s">
         <v>290</v>
@@ -4284,7 +4294,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="308" customHeight="1" ht="18.75">
       <c r="A308" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B308" s="5" t="s">
         <v>291</v>
@@ -4293,7 +4303,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="309" customHeight="1" ht="18.75">
       <c r="A309" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B309" s="5" t="s">
         <v>292</v>
@@ -4302,7 +4312,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="310" customHeight="1" ht="18.75">
       <c r="A310" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B310" s="5" t="s">
         <v>293</v>
@@ -4311,7 +4321,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="311" customHeight="1" ht="18.75">
       <c r="A311" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B311" s="5" t="s">
         <v>294</v>
@@ -4320,7 +4330,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="312" customHeight="1" ht="18.75">
       <c r="A312" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B312" s="5" t="s">
         <v>295</v>
@@ -4329,7 +4339,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="313" customHeight="1" ht="18.75">
       <c r="A313" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B313" s="5" t="s">
         <v>296</v>
@@ -4338,7 +4348,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="314" customHeight="1" ht="18.75">
       <c r="A314" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B314" s="5" t="s">
         <v>297</v>
@@ -4346,9 +4356,13 @@
       <c r="C314" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="315" customHeight="1" ht="18.75">
-      <c r="A315" s="4"/>
-      <c r="B315" s="7"/>
-      <c r="C315" s="8"/>
+      <c r="A315" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B315" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C315" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="316" customHeight="1" ht="18.75">
       <c r="A316" s="4"/>
@@ -4357,19 +4371,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="317" customHeight="1" ht="18.75">
       <c r="A317" s="4"/>
-      <c r="B317" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="C317" s="13"/>
+      <c r="B317" s="7"/>
+      <c r="C317" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="318" customHeight="1" ht="18.75">
-      <c r="A318" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B318" s="5" t="s">
+      <c r="A318" s="4"/>
+      <c r="B318" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="C318" s="6"/>
+      <c r="C318" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="319" customHeight="1" ht="18.75">
       <c r="A319" s="4" t="s">
@@ -4436,7 +4446,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="326" customHeight="1" ht="18.75">
       <c r="A326" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B326" s="5" t="s">
         <v>307</v>
@@ -4445,7 +4455,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="327" customHeight="1" ht="18.75">
       <c r="A327" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B327" s="5" t="s">
         <v>308</v>
@@ -4454,7 +4464,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="328" customHeight="1" ht="18.75">
       <c r="A328" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B328" s="5" t="s">
         <v>309</v>
@@ -4463,7 +4473,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="329" customHeight="1" ht="18.75">
       <c r="A329" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B329" s="5" t="s">
         <v>310</v>
@@ -4472,7 +4482,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="330" customHeight="1" ht="18.75">
       <c r="A330" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B330" s="5" t="s">
         <v>311</v>
@@ -4481,7 +4491,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="331" customHeight="1" ht="18.75">
       <c r="A331" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B331" s="5" t="s">
         <v>312</v>
@@ -4490,7 +4500,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="332" customHeight="1" ht="18.75">
       <c r="A332" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B332" s="5" t="s">
         <v>313</v>
@@ -4499,7 +4509,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="333" customHeight="1" ht="18.75">
       <c r="A333" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B333" s="5" t="s">
         <v>314</v>
@@ -4508,7 +4518,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="334" customHeight="1" ht="18.75">
       <c r="A334" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B334" s="5" t="s">
         <v>315</v>
@@ -4517,7 +4527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="335" customHeight="1" ht="18.75">
       <c r="A335" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B335" s="5" t="s">
         <v>316</v>
@@ -4525,29 +4535,29 @@
       <c r="C335" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="336" customHeight="1" ht="18.75">
-      <c r="A336" s="4"/>
-      <c r="B336" s="7"/>
-      <c r="C336" s="8"/>
+      <c r="A336" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B336" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C336" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="337" customHeight="1" ht="18.75">
       <c r="A337" s="4"/>
-      <c r="B337" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="C337" s="17"/>
+      <c r="B337" s="7"/>
+      <c r="C337" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="338" customHeight="1" ht="18.75">
-      <c r="A338" s="4" t="s">
+      <c r="A338" s="4"/>
+      <c r="B338" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="B338" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C338" s="6"/>
+      <c r="C338" s="18"/>
     </row>
     <row x14ac:dyDescent="0.25" r="339" customHeight="1" ht="18.75">
       <c r="A339" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B339" s="5" t="s">
         <v>320</v>
@@ -4556,26 +4566,30 @@
     </row>
     <row x14ac:dyDescent="0.25" r="340" customHeight="1" ht="18.75">
       <c r="A340" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>89</v>
+        <v>321</v>
       </c>
       <c r="C340" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="341" customHeight="1" ht="18.75">
       <c r="A341" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B341" s="5" t="s">
-        <v>321</v>
+        <v>90</v>
       </c>
       <c r="C341" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="342" customHeight="1" ht="18.75">
-      <c r="A342" s="4"/>
-      <c r="B342" s="7"/>
-      <c r="C342" s="8"/>
+      <c r="A342" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B342" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C342" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="343" customHeight="1" ht="18.75">
       <c r="A343" s="4"/>
@@ -7868,9 +7882,14 @@
       <c r="C1000" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1001" customHeight="1" ht="18.75">
-      <c r="A1001" s="18"/>
-      <c r="B1001" s="19"/>
+      <c r="A1001" s="4"/>
+      <c r="B1001" s="7"/>
       <c r="C1001" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="1002" customHeight="1" ht="18.75">
+      <c r="A1002" s="19"/>
+      <c r="B1002" s="20"/>
+      <c r="C1002" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add HappyNumber class to determine if a number is a happy number
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -990,7 +990,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,6 +1023,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1209,10 +1215,10 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -1227,16 +1233,16 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -2237,7 +2243,9 @@
       <c r="B70" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="6"/>
+      <c r="C70" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="4" t="s">

</xml_diff>

<commit_message>
Add IsPalindrome class to check if a number is a palindrome
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2254,7 +2254,9 @@
       <c r="B71" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="6"/>
+      <c r="C71" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="4" t="s">

</xml_diff>

<commit_message>
Add MissingNumber class to find the missing number in an array
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2265,7 +2265,9 @@
       <c r="B72" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="6"/>
+      <c r="C72" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="4" t="s">

</xml_diff>

<commit_message>
Add ReverseInteger class to reverse an integer and handle overflow
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2271,12 +2271,14 @@
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="6"/>
+      <c r="C73" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="4" t="s">

</xml_diff>

<commit_message>
Add PowerOfTwo class to determine if a number is a power of two
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="323">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -990,7 +990,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,12 +1023,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1189,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1218,9 +1212,6 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1233,16 +1224,16 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -1562,9 +1553,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="98.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="98.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2167,9 +2158,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="4" t="s">
@@ -2287,7 +2278,9 @@
       <c r="B74" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="6"/>
+      <c r="C74" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="4" t="s">
@@ -2377,10 +2370,10 @@
       <c r="A85" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C85" s="12"/>
+      <c r="C85" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="4" t="s">
@@ -2395,19 +2388,19 @@
       <c r="A87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="12"/>
+      <c r="C87" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C88" s="12"/>
+      <c r="C88" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="4" t="s">
@@ -2440,28 +2433,28 @@
       <c r="A92" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="12"/>
+      <c r="C92" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="12"/>
+      <c r="C93" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="12"/>
+      <c r="C94" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="4"/>
@@ -2475,10 +2468,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="4"/>
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C97" s="14"/>
+      <c r="C97" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="4" t="s">
@@ -2757,10 +2750,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="4"/>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C129" s="14"/>
+      <c r="C129" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="4"/>
@@ -2959,10 +2952,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="4"/>
-      <c r="B153" s="15" t="s">
+      <c r="B153" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C153" s="16"/>
+      <c r="C153" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="4" t="s">
@@ -3814,10 +3807,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="18.75">
       <c r="A250" s="4"/>
-      <c r="B250" s="13" t="s">
+      <c r="B250" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="C250" s="14"/>
+      <c r="C250" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="18.75">
       <c r="A251" s="4"/>
@@ -4390,10 +4383,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="318" customHeight="1" ht="18.75">
       <c r="A318" s="4"/>
-      <c r="B318" s="13" t="s">
+      <c r="B318" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="C318" s="14"/>
+      <c r="C318" s="13"/>
     </row>
     <row x14ac:dyDescent="0.25" r="319" customHeight="1" ht="18.75">
       <c r="A319" s="4" t="s">
@@ -4564,10 +4557,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="338" customHeight="1" ht="18.75">
       <c r="A338" s="4"/>
-      <c r="B338" s="17" t="s">
+      <c r="B338" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="C338" s="18"/>
+      <c r="C338" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="339" customHeight="1" ht="18.75">
       <c r="A339" s="4" t="s">
@@ -7901,8 +7894,8 @@
       <c r="C1001" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1002" customHeight="1" ht="18.75">
-      <c r="A1002" s="19"/>
-      <c r="B1002" s="20"/>
+      <c r="A1002" s="18"/>
+      <c r="B1002" s="19"/>
       <c r="C1002" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add HCF and LCM calculations, and implement KthFactor method to find the k-th factor of a number
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/the-kth-factor-of-n/</t>
+  </si>
+  <si>
+    <t>hcf and lcm</t>
   </si>
   <si>
     <t>Sorting and Searching</t>
@@ -2307,17 +2310,23 @@
       <c r="B77" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="6"/>
+      <c r="C77" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="4"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="8"/>
+      <c r="B78" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="4"/>
       <c r="B79" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C79" s="8"/>
     </row>
@@ -2326,7 +2335,7 @@
         <v>9</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C80" s="6"/>
     </row>
@@ -2335,7 +2344,7 @@
         <v>9</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C81" s="6"/>
     </row>
@@ -2344,7 +2353,7 @@
         <v>9</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C82" s="6"/>
     </row>
@@ -2353,7 +2362,7 @@
         <v>9</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C83" s="6"/>
     </row>
@@ -2362,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C84" s="6"/>
     </row>
@@ -2371,7 +2380,7 @@
         <v>5</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C85" s="11"/>
     </row>
@@ -2380,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C86" s="6"/>
     </row>
@@ -2389,7 +2398,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C87" s="11"/>
     </row>
@@ -2398,7 +2407,7 @@
         <v>5</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C88" s="11"/>
     </row>
@@ -2407,7 +2416,7 @@
         <v>34</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C89" s="6"/>
     </row>
@@ -2416,7 +2425,7 @@
         <v>34</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C90" s="6"/>
     </row>
@@ -2425,7 +2434,7 @@
         <v>34</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C91" s="6"/>
     </row>
@@ -2434,7 +2443,7 @@
         <v>34</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C92" s="11"/>
     </row>
@@ -2443,7 +2452,7 @@
         <v>34</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C93" s="11"/>
     </row>
@@ -2452,7 +2461,7 @@
         <v>34</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C94" s="11"/>
     </row>
@@ -2469,7 +2478,7 @@
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C97" s="13"/>
     </row>
@@ -2478,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C98" s="6"/>
     </row>
@@ -2487,7 +2496,7 @@
         <v>9</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C99" s="6"/>
     </row>
@@ -2496,7 +2505,7 @@
         <v>9</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C100" s="6"/>
     </row>
@@ -2505,7 +2514,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C101" s="6"/>
     </row>
@@ -2514,7 +2523,7 @@
         <v>9</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C102" s="6"/>
     </row>
@@ -2523,7 +2532,7 @@
         <v>9</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C103" s="6"/>
     </row>
@@ -2532,7 +2541,7 @@
         <v>9</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C104" s="6"/>
     </row>
@@ -2541,7 +2550,7 @@
         <v>9</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C105" s="6"/>
     </row>
@@ -2550,7 +2559,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C106" s="6"/>
     </row>
@@ -2559,7 +2568,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C107" s="6"/>
     </row>
@@ -2568,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C108" s="6"/>
     </row>
@@ -2577,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C109" s="6"/>
     </row>
@@ -2586,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C110" s="6"/>
     </row>
@@ -2595,7 +2604,7 @@
         <v>5</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C111" s="6"/>
     </row>
@@ -2604,7 +2613,7 @@
         <v>5</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C112" s="6"/>
     </row>
@@ -2613,7 +2622,7 @@
         <v>5</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C113" s="6"/>
     </row>
@@ -2622,7 +2631,7 @@
         <v>5</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C114" s="6"/>
     </row>
@@ -2631,7 +2640,7 @@
         <v>5</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C115" s="6"/>
     </row>
@@ -2640,7 +2649,7 @@
         <v>5</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C116" s="6"/>
     </row>
@@ -2649,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C117" s="6"/>
     </row>
@@ -2658,7 +2667,7 @@
         <v>5</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C118" s="6"/>
     </row>
@@ -2667,7 +2676,7 @@
         <v>5</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C119" s="6"/>
     </row>
@@ -2676,7 +2685,7 @@
         <v>5</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C120" s="6"/>
     </row>
@@ -2685,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C121" s="6"/>
     </row>
@@ -2694,7 +2703,7 @@
         <v>5</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C122" s="6"/>
     </row>
@@ -2703,7 +2712,7 @@
         <v>34</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C123" s="6"/>
     </row>
@@ -2712,7 +2721,7 @@
         <v>34</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C124" s="6"/>
     </row>
@@ -2721,7 +2730,7 @@
         <v>34</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C125" s="6"/>
     </row>
@@ -2730,7 +2739,7 @@
         <v>34</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C126" s="6"/>
     </row>
@@ -2739,7 +2748,7 @@
         <v>34</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C127" s="6"/>
     </row>
@@ -2751,7 +2760,7 @@
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="4"/>
       <c r="B129" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C129" s="13"/>
     </row>
@@ -2765,7 +2774,7 @@
         <v>9</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C131" s="6"/>
     </row>
@@ -2774,7 +2783,7 @@
         <v>9</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C132" s="6"/>
     </row>
@@ -2783,7 +2792,7 @@
         <v>9</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C133" s="6"/>
     </row>
@@ -2792,7 +2801,7 @@
         <v>9</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C134" s="6"/>
     </row>
@@ -2801,7 +2810,7 @@
         <v>9</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C135" s="6"/>
     </row>
@@ -2810,7 +2819,7 @@
         <v>9</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C136" s="6"/>
     </row>
@@ -2819,7 +2828,7 @@
         <v>9</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C137" s="6"/>
     </row>
@@ -2828,7 +2837,7 @@
         <v>5</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C138" s="6"/>
     </row>
@@ -2837,7 +2846,7 @@
         <v>5</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C139" s="6"/>
     </row>
@@ -2846,7 +2855,7 @@
         <v>5</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C140" s="6"/>
     </row>
@@ -2855,7 +2864,7 @@
         <v>5</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C141" s="6"/>
     </row>
@@ -2864,7 +2873,7 @@
         <v>5</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C142" s="6"/>
     </row>
@@ -2873,7 +2882,7 @@
         <v>5</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C143" s="6"/>
     </row>
@@ -2882,7 +2891,7 @@
         <v>5</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C144" s="6"/>
     </row>
@@ -2891,7 +2900,7 @@
         <v>5</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C145" s="6"/>
     </row>
@@ -2900,7 +2909,7 @@
         <v>5</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C146" s="6"/>
     </row>
@@ -2909,7 +2918,7 @@
         <v>5</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C147" s="6"/>
     </row>
@@ -2918,7 +2927,7 @@
         <v>34</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C148" s="6"/>
     </row>
@@ -2927,7 +2936,7 @@
         <v>34</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C149" s="6"/>
     </row>
@@ -2936,7 +2945,7 @@
         <v>34</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C150" s="6"/>
     </row>
@@ -2953,7 +2962,7 @@
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C153" s="15"/>
     </row>
@@ -2962,7 +2971,7 @@
         <v>9</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C154" s="6"/>
     </row>
@@ -2971,7 +2980,7 @@
         <v>9</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C155" s="6"/>
     </row>
@@ -2980,7 +2989,7 @@
         <v>9</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C156" s="6"/>
     </row>
@@ -2989,7 +2998,7 @@
         <v>9</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C157" s="6"/>
     </row>
@@ -2998,7 +3007,7 @@
         <v>9</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C158" s="6"/>
     </row>
@@ -3007,7 +3016,7 @@
         <v>9</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C159" s="6"/>
     </row>
@@ -3016,7 +3025,7 @@
         <v>9</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C160" s="6"/>
     </row>
@@ -3025,7 +3034,7 @@
         <v>9</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C161" s="6"/>
     </row>
@@ -3034,7 +3043,7 @@
         <v>9</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C162" s="6"/>
     </row>
@@ -3043,7 +3052,7 @@
         <v>9</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C163" s="6"/>
     </row>
@@ -3052,7 +3061,7 @@
         <v>9</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C164" s="6"/>
     </row>
@@ -3061,7 +3070,7 @@
         <v>9</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C165" s="6"/>
     </row>
@@ -3070,7 +3079,7 @@
         <v>9</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C166" s="6"/>
     </row>
@@ -3079,7 +3088,7 @@
         <v>9</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C167" s="6"/>
     </row>
@@ -3088,7 +3097,7 @@
         <v>9</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C168" s="6"/>
     </row>
@@ -3097,7 +3106,7 @@
         <v>9</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C169" s="6"/>
     </row>
@@ -3106,7 +3115,7 @@
         <v>9</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C170" s="6"/>
     </row>
@@ -3115,7 +3124,7 @@
         <v>9</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C171" s="6"/>
     </row>
@@ -3124,7 +3133,7 @@
         <v>5</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C172" s="6"/>
     </row>
@@ -3133,7 +3142,7 @@
         <v>5</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C173" s="6"/>
     </row>
@@ -3142,7 +3151,7 @@
         <v>5</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C174" s="6"/>
     </row>
@@ -3151,7 +3160,7 @@
         <v>5</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C175" s="6"/>
     </row>
@@ -3160,7 +3169,7 @@
         <v>5</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C176" s="6"/>
     </row>
@@ -3169,7 +3178,7 @@
         <v>5</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C177" s="6"/>
     </row>
@@ -3178,7 +3187,7 @@
         <v>5</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C178" s="6"/>
     </row>
@@ -3187,7 +3196,7 @@
         <v>5</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C179" s="6"/>
     </row>
@@ -3196,7 +3205,7 @@
         <v>5</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C180" s="6"/>
     </row>
@@ -3205,7 +3214,7 @@
         <v>5</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C181" s="6"/>
     </row>
@@ -3214,7 +3223,7 @@
         <v>5</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C182" s="6"/>
     </row>
@@ -3223,7 +3232,7 @@
         <v>5</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C183" s="6"/>
     </row>
@@ -3232,7 +3241,7 @@
         <v>5</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C184" s="6"/>
     </row>
@@ -3241,7 +3250,7 @@
         <v>5</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C185" s="6"/>
     </row>
@@ -3250,7 +3259,7 @@
         <v>5</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C186" s="6"/>
     </row>
@@ -3259,7 +3268,7 @@
         <v>5</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C187" s="6"/>
     </row>
@@ -3268,7 +3277,7 @@
         <v>5</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C188" s="6"/>
     </row>
@@ -3277,7 +3286,7 @@
         <v>5</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C189" s="6"/>
     </row>
@@ -3286,7 +3295,7 @@
         <v>5</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C190" s="6"/>
     </row>
@@ -3295,7 +3304,7 @@
         <v>5</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C191" s="6"/>
     </row>
@@ -3304,7 +3313,7 @@
         <v>34</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C192" s="6"/>
     </row>
@@ -3313,7 +3322,7 @@
         <v>34</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C193" s="6"/>
     </row>
@@ -3322,7 +3331,7 @@
         <v>34</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C194" s="6"/>
     </row>
@@ -3331,7 +3340,7 @@
         <v>34</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C195" s="6"/>
     </row>
@@ -3340,7 +3349,7 @@
         <v>34</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C196" s="6"/>
     </row>
@@ -3349,7 +3358,7 @@
         <v>34</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C197" s="6"/>
     </row>
@@ -3358,7 +3367,7 @@
         <v>34</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C198" s="6"/>
     </row>
@@ -3367,7 +3376,7 @@
         <v>34</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C199" s="6"/>
     </row>
@@ -3376,7 +3385,7 @@
         <v>34</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C200" s="6"/>
     </row>
@@ -3385,7 +3394,7 @@
         <v>34</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C201" s="6"/>
     </row>
@@ -3397,7 +3406,7 @@
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
       <c r="A203" s="4"/>
       <c r="B203" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C203" s="8"/>
     </row>
@@ -3406,7 +3415,7 @@
         <v>9</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C204" s="6"/>
     </row>
@@ -3415,7 +3424,7 @@
         <v>9</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C205" s="6"/>
     </row>
@@ -3424,7 +3433,7 @@
         <v>9</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C206" s="6"/>
     </row>
@@ -3433,7 +3442,7 @@
         <v>9</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C207" s="6"/>
     </row>
@@ -3442,7 +3451,7 @@
         <v>9</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C208" s="6"/>
     </row>
@@ -3451,7 +3460,7 @@
         <v>9</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C209" s="6"/>
     </row>
@@ -3460,7 +3469,7 @@
         <v>9</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C210" s="6"/>
     </row>
@@ -3469,7 +3478,7 @@
         <v>5</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C211" s="6"/>
     </row>
@@ -3478,7 +3487,7 @@
         <v>5</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C212" s="6"/>
     </row>
@@ -3487,7 +3496,7 @@
         <v>5</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C213" s="6"/>
     </row>
@@ -3496,7 +3505,7 @@
         <v>5</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C214" s="6"/>
     </row>
@@ -3505,7 +3514,7 @@
         <v>5</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C215" s="6"/>
     </row>
@@ -3514,7 +3523,7 @@
         <v>5</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C216" s="6"/>
     </row>
@@ -3523,7 +3532,7 @@
         <v>5</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C217" s="6"/>
     </row>
@@ -3532,7 +3541,7 @@
         <v>5</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C218" s="6"/>
     </row>
@@ -3541,7 +3550,7 @@
         <v>5</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C219" s="6"/>
     </row>
@@ -3550,7 +3559,7 @@
         <v>5</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C220" s="6"/>
     </row>
@@ -3559,7 +3568,7 @@
         <v>5</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C221" s="6"/>
     </row>
@@ -3568,7 +3577,7 @@
         <v>5</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C222" s="6"/>
     </row>
@@ -3577,7 +3586,7 @@
         <v>5</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C223" s="6"/>
     </row>
@@ -3586,7 +3595,7 @@
         <v>5</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C224" s="6"/>
     </row>
@@ -3595,7 +3604,7 @@
         <v>5</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C225" s="6"/>
     </row>
@@ -3604,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C226" s="6"/>
     </row>
@@ -3613,7 +3622,7 @@
         <v>5</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C227" s="6"/>
     </row>
@@ -3622,7 +3631,7 @@
         <v>5</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C228" s="6"/>
     </row>
@@ -3631,7 +3640,7 @@
         <v>5</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C229" s="6"/>
     </row>
@@ -3640,7 +3649,7 @@
         <v>5</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C230" s="6"/>
     </row>
@@ -3649,7 +3658,7 @@
         <v>34</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C231" s="6"/>
     </row>
@@ -3658,7 +3667,7 @@
         <v>34</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C232" s="6"/>
     </row>
@@ -3667,7 +3676,7 @@
         <v>34</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C233" s="6"/>
     </row>
@@ -3676,7 +3685,7 @@
         <v>34</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C234" s="6"/>
     </row>
@@ -3685,7 +3694,7 @@
         <v>34</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C235" s="6"/>
     </row>
@@ -3694,7 +3703,7 @@
         <v>34</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C236" s="6"/>
     </row>
@@ -3703,7 +3712,7 @@
         <v>34</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C237" s="6"/>
     </row>
@@ -3712,7 +3721,7 @@
         <v>34</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C238" s="6"/>
     </row>
@@ -3721,7 +3730,7 @@
         <v>34</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C239" s="6"/>
     </row>
@@ -3730,7 +3739,7 @@
         <v>34</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C240" s="6"/>
     </row>
@@ -3742,7 +3751,7 @@
     <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="18.75">
       <c r="A242" s="4"/>
       <c r="B242" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C242" s="8"/>
     </row>
@@ -3751,7 +3760,7 @@
         <v>5</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C243" s="6"/>
     </row>
@@ -3760,7 +3769,7 @@
         <v>5</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C244" s="6"/>
     </row>
@@ -3769,7 +3778,7 @@
         <v>5</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C245" s="6"/>
     </row>
@@ -3778,7 +3787,7 @@
         <v>5</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C246" s="6"/>
     </row>
@@ -3787,7 +3796,7 @@
         <v>34</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C247" s="6"/>
     </row>
@@ -3796,7 +3805,7 @@
         <v>34</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C248" s="6"/>
     </row>
@@ -3808,7 +3817,7 @@
     <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="18.75">
       <c r="A250" s="4"/>
       <c r="B250" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C250" s="13"/>
     </row>
@@ -3819,91 +3828,91 @@
     </row>
     <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="18.75">
       <c r="A252" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C252" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18.75">
       <c r="A253" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C253" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="18.75">
       <c r="A254" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C254" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="18.75">
       <c r="A255" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C255" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="18.75">
       <c r="A256" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C256" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="18.75">
       <c r="A257" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C257" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="18.75">
       <c r="A258" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C258" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="18.75">
       <c r="A259" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C259" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="18.75">
       <c r="A260" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C260" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="18.75">
       <c r="A261" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C261" s="6"/>
     </row>
@@ -3912,7 +3921,7 @@
         <v>34</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C262" s="6"/>
     </row>
@@ -3921,7 +3930,7 @@
         <v>34</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C263" s="6"/>
     </row>
@@ -3930,7 +3939,7 @@
         <v>34</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C264" s="6"/>
     </row>
@@ -3939,7 +3948,7 @@
         <v>34</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C265" s="6"/>
     </row>
@@ -3951,7 +3960,7 @@
     <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="18.75">
       <c r="A267" s="4"/>
       <c r="B267" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C267" s="8"/>
     </row>
@@ -3960,7 +3969,7 @@
         <v>9</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C268" s="6"/>
     </row>
@@ -3969,7 +3978,7 @@
         <v>9</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C269" s="6"/>
     </row>
@@ -3978,7 +3987,7 @@
         <v>9</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C270" s="6"/>
     </row>
@@ -3987,7 +3996,7 @@
         <v>9</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C271" s="6"/>
     </row>
@@ -3996,7 +4005,7 @@
         <v>5</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C272" s="6"/>
     </row>
@@ -4005,7 +4014,7 @@
         <v>5</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C273" s="6"/>
     </row>
@@ -4014,7 +4023,7 @@
         <v>5</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C274" s="6"/>
     </row>
@@ -4023,7 +4032,7 @@
         <v>5</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C275" s="6"/>
     </row>
@@ -4032,7 +4041,7 @@
         <v>5</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C276" s="6"/>
     </row>
@@ -4041,7 +4050,7 @@
         <v>5</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C277" s="6"/>
     </row>
@@ -4050,7 +4059,7 @@
         <v>5</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C278" s="6"/>
     </row>
@@ -4059,7 +4068,7 @@
         <v>5</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C279" s="6"/>
     </row>
@@ -4068,7 +4077,7 @@
         <v>5</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C280" s="6"/>
     </row>
@@ -4077,7 +4086,7 @@
         <v>5</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C281" s="6"/>
     </row>
@@ -4086,7 +4095,7 @@
         <v>5</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C282" s="6"/>
     </row>
@@ -4095,7 +4104,7 @@
         <v>5</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C283" s="6"/>
     </row>
@@ -4104,7 +4113,7 @@
         <v>5</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C284" s="6"/>
     </row>
@@ -4113,7 +4122,7 @@
         <v>5</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C285" s="6"/>
     </row>
@@ -4122,7 +4131,7 @@
         <v>5</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C286" s="6"/>
     </row>
@@ -4131,7 +4140,7 @@
         <v>34</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C287" s="6"/>
     </row>
@@ -4140,7 +4149,7 @@
         <v>34</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C288" s="6"/>
     </row>
@@ -4149,7 +4158,7 @@
         <v>34</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C289" s="6"/>
     </row>
@@ -4158,7 +4167,7 @@
         <v>34</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C290" s="6"/>
     </row>
@@ -4167,7 +4176,7 @@
         <v>34</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C291" s="6"/>
     </row>
@@ -4176,7 +4185,7 @@
         <v>34</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C292" s="6"/>
     </row>
@@ -4185,7 +4194,7 @@
         <v>34</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C293" s="6"/>
     </row>
@@ -4194,7 +4203,7 @@
         <v>34</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C294" s="6"/>
     </row>
@@ -4203,7 +4212,7 @@
         <v>34</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C295" s="6"/>
     </row>
@@ -4212,7 +4221,7 @@
         <v>34</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C296" s="6"/>
     </row>
@@ -4221,7 +4230,7 @@
         <v>34</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C297" s="6"/>
     </row>
@@ -4233,7 +4242,7 @@
     <row x14ac:dyDescent="0.25" r="299" customHeight="1" ht="18.75">
       <c r="A299" s="4"/>
       <c r="B299" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C299" s="8"/>
     </row>
@@ -4251,7 +4260,7 @@
         <v>5</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C301" s="6"/>
     </row>
@@ -4260,7 +4269,7 @@
         <v>5</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C302" s="6"/>
     </row>
@@ -4277,97 +4286,97 @@
     <row x14ac:dyDescent="0.25" r="305" customHeight="1" ht="18.75">
       <c r="A305" s="4"/>
       <c r="B305" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C305" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="306" customHeight="1" ht="18.75">
       <c r="A306" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C306" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="307" customHeight="1" ht="18.75">
       <c r="A307" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C307" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="308" customHeight="1" ht="18.75">
       <c r="A308" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C308" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="309" customHeight="1" ht="18.75">
       <c r="A309" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C309" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="310" customHeight="1" ht="18.75">
       <c r="A310" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C310" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="311" customHeight="1" ht="18.75">
       <c r="A311" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C311" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="312" customHeight="1" ht="18.75">
       <c r="A312" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C312" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="313" customHeight="1" ht="18.75">
       <c r="A313" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C313" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="314" customHeight="1" ht="18.75">
       <c r="A314" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C314" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="315" customHeight="1" ht="18.75">
       <c r="A315" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C315" s="6"/>
     </row>
@@ -4384,7 +4393,7 @@
     <row x14ac:dyDescent="0.25" r="318" customHeight="1" ht="18.75">
       <c r="A318" s="4"/>
       <c r="B318" s="12" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C318" s="13"/>
     </row>
@@ -4393,7 +4402,7 @@
         <v>5</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C319" s="6"/>
     </row>
@@ -4402,7 +4411,7 @@
         <v>5</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C320" s="6"/>
     </row>
@@ -4411,7 +4420,7 @@
         <v>5</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C321" s="6"/>
     </row>
@@ -4420,7 +4429,7 @@
         <v>5</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C322" s="6"/>
     </row>
@@ -4429,7 +4438,7 @@
         <v>5</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C323" s="6"/>
     </row>
@@ -4438,7 +4447,7 @@
         <v>5</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C324" s="6"/>
     </row>
@@ -4447,7 +4456,7 @@
         <v>5</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C325" s="6"/>
     </row>
@@ -4456,7 +4465,7 @@
         <v>5</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C326" s="6"/>
     </row>
@@ -4465,7 +4474,7 @@
         <v>34</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C327" s="6"/>
     </row>
@@ -4474,7 +4483,7 @@
         <v>34</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C328" s="6"/>
     </row>
@@ -4483,7 +4492,7 @@
         <v>34</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C329" s="6"/>
     </row>
@@ -4492,7 +4501,7 @@
         <v>34</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C330" s="6"/>
     </row>
@@ -4501,7 +4510,7 @@
         <v>34</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C331" s="6"/>
     </row>
@@ -4510,7 +4519,7 @@
         <v>34</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C332" s="6"/>
     </row>
@@ -4519,7 +4528,7 @@
         <v>34</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C333" s="6"/>
     </row>
@@ -4528,7 +4537,7 @@
         <v>34</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C334" s="6"/>
     </row>
@@ -4537,7 +4546,7 @@
         <v>34</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C335" s="6"/>
     </row>
@@ -4546,7 +4555,7 @@
         <v>34</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C336" s="6"/>
     </row>
@@ -4558,43 +4567,43 @@
     <row x14ac:dyDescent="0.25" r="338" customHeight="1" ht="18.75">
       <c r="A338" s="4"/>
       <c r="B338" s="16" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C338" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="339" customHeight="1" ht="18.75">
       <c r="A339" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C339" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="340" customHeight="1" ht="18.75">
       <c r="A340" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C340" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="341" customHeight="1" ht="18.75">
       <c r="A341" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B341" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C341" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="342" customHeight="1" ht="18.75">
       <c r="A342" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C342" s="6"/>
     </row>

</xml_diff>

<commit_message>
Add new searching and sorting algorithms: CeilingOfANumber, PairDifference, and ReversingSubArrayToSort
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1579,12 +1579,12 @@
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
@@ -2346,7 +2346,9 @@
       <c r="B81" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="6"/>
+      <c r="C81" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="4" t="s">

</xml_diff>

<commit_message>
Add binary search algorithms: FindPeakElement and SearchInRotatedSortedArray implementations
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2176,12 +2176,12 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
       <c r="A64" s="4"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
       <c r="A65" s="4"/>
       <c r="B65" s="7" t="s">
         <v>64</v>
@@ -2314,7 +2314,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
       <c r="A78" s="4"/>
       <c r="B78" s="7" t="s">
         <v>77</v>
@@ -2384,7 +2384,9 @@
       <c r="B85" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="11"/>
+      <c r="C85" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="4" t="s">
@@ -2411,7 +2413,9 @@
       <c r="B88" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="11"/>
+      <c r="C88" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="4" t="s">
@@ -2447,7 +2451,9 @@
       <c r="B92" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="11"/>
+      <c r="C92" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="4" t="s">

</xml_diff>

<commit_message>
Add merge sort implementation to CountSmaller class
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -2473,17 +2473,17 @@
       </c>
       <c r="C94" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
       <c r="A95" s="4"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
       <c r="A96" s="4"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
Add HasCycle class to detect cycles in a linked list using the two-pointer approach
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2473,17 +2473,17 @@
       </c>
       <c r="C94" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="4"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="4"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
         <v>93</v>
@@ -2497,7 +2497,9 @@
       <c r="B98" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C98" s="6"/>
+      <c r="C98" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="4" t="s">
@@ -2506,7 +2508,9 @@
       <c r="B99" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C99" s="6"/>
+      <c r="C99" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="4" t="s">

</xml_diff>

<commit_message>
Add BinaryToDecimal and GenericConversion classes for binary to decimal conversion
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2519,7 +2519,9 @@
       <c r="B100" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="6"/>
+      <c r="C100" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="4" t="s">

</xml_diff>

<commit_message>
Add RemoveDuplicates class to delete duplicates from a sorted linked list
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2530,7 +2530,9 @@
       <c r="B101" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="6"/>
+      <c r="C101" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="4" t="s">

</xml_diff>

<commit_message>
Add ListNode and RemoveVal classes for linked list element removal
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2483,7 +2483,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
         <v>93</v>
@@ -2550,7 +2550,9 @@
       <c r="B103" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="6"/>
+      <c r="C103" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="4" t="s">

</xml_diff>

<commit_message>
Refactor MergeSort implementation and add detailed documentation for merging two sorted linked lists
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2483,7 +2483,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
         <v>93</v>
@@ -2561,7 +2561,9 @@
       <c r="B104" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="6"/>
+      <c r="C104" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="4" t="s">

</xml_diff>

<commit_message>
Add ReverseLinkedList class to implement linked list reversal using a stack
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2483,7 +2483,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
         <v>93</v>
@@ -2581,7 +2581,9 @@
       <c r="B106" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="6"/>
+      <c r="C106" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="4" t="s">
@@ -2599,7 +2601,9 @@
       <c r="B108" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="6"/>
+      <c r="C108" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="4" t="s">
@@ -2608,7 +2612,9 @@
       <c r="B109" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C109" s="6"/>
+      <c r="C109" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="4" t="s">

</xml_diff>

<commit_message>
Add Node class to implement linked list with random pointers and utility methods
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2623,7 +2623,9 @@
       <c r="B110" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C110" s="6"/>
+      <c r="C110" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="4" t="s">

</xml_diff>

<commit_message>
Enhance copyRandomList method to create a deep copy of linked list with random pointers and improve documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2483,7 +2483,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="4"/>
       <c r="B97" s="12" t="s">
         <v>93</v>
@@ -2634,7 +2634,9 @@
       <c r="B111" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C111" s="6"/>
+      <c r="C111" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="4" t="s">

</xml_diff>

<commit_message>
Add AddTwoNumber2 class to sum two linked lists with digits stored in reverse order and enhance documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2645,7 +2645,9 @@
       <c r="B112" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C112" s="6"/>
+      <c r="C112" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="4" t="s">

</xml_diff>

<commit_message>
Add ReverseLinkedList2 class to reverse a portion of a linked list between given indices
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2656,7 +2656,9 @@
       <c r="B113" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C113" s="6"/>
+      <c r="C113" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="4" t="s">

</xml_diff>

<commit_message>
Enhance ReOrderList class to improve the reorder logic and add detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2667,7 +2667,9 @@
       <c r="B114" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C114" s="6"/>
+      <c r="C114" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="4" t="s">

</xml_diff>

<commit_message>
Add RemoveNthFromLast class to remove the nth node from the end of a linked list with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2678,7 +2678,9 @@
       <c r="B115" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C115" s="6"/>
+      <c r="C115" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="4" t="s">

</xml_diff>

<commit_message>
Add FlattenList class to flatten a multilevel doubly linked list with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2689,7 +2689,9 @@
       <c r="B116" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C116" s="6"/>
+      <c r="C116" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="4" t="s">

</xml_diff>

<commit_message>
Add PartitionList class to partition a linked list around a value with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2700,7 +2700,9 @@
       <c r="B117" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C117" s="6"/>
+      <c r="C117" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="4" t="s">

</xml_diff>

<commit_message>
Add RemoveDuplicates2 class to remove duplicates from a sorted linked list while keeping only unique elements with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2711,7 +2711,9 @@
       <c r="B118" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C118" s="6"/>
+      <c r="C118" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="4" t="s">

</xml_diff>

<commit_message>
Enhance SortLists class with detailed Merge Sort algorithm documentation and remove debug print statements
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2731,7 +2731,9 @@
       <c r="B120" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C120" s="6"/>
+      <c r="C120" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="4" t="s">

</xml_diff>

<commit_message>
Add MergeKSortedLists class to merge k sorted linked lists with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2760,7 +2760,9 @@
       <c r="B123" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C123" s="6"/>
+      <c r="C123" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="4" t="s">

</xml_diff>

<commit_message>
Add ReverseKPart class to reverse nodes in k-group in a linked list with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2771,7 +2771,9 @@
       <c r="B124" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C124" s="6"/>
+      <c r="C124" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="4" t="s">

</xml_diff>

<commit_message>
Add QueueFromStack class to implement a queue using two stacks
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2826,7 +2826,9 @@
       <c r="B131" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C131" s="6"/>
+      <c r="C131" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="4" t="s">

</xml_diff>

<commit_message>
Add StackFromQueue class to implement a stack using a queue with detailed documentation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2837,7 +2837,9 @@
       <c r="B132" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C132" s="6"/>
+      <c r="C132" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="4" t="s">
@@ -2846,7 +2848,9 @@
       <c r="B133" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C133" s="6"/>
+      <c r="C133" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="4" t="s">

</xml_diff>

<commit_message>
Add NextGreaterElement class to find the next greater element for each element in an array
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2868,7 +2868,9 @@
       <c r="B135" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C135" s="6"/>
+      <c r="C135" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="4" t="s">

</xml_diff>

<commit_message>
Add DailyTemps class to calculate the number of days until a warmer temperature
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2906,7 +2906,9 @@
       <c r="B139" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C139" s="6"/>
+      <c r="C139" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="4" t="s">

</xml_diff>

<commit_message>
Add RPN class to evaluate expressions in Reverse Polish Notation
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2953,7 +2953,9 @@
       <c r="B144" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C144" s="6"/>
+      <c r="C144" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="4" t="s">

</xml_diff>

<commit_message>
Add RemoveAdjacentDups2 class to solve LeetCode problem 1209 using a stack-based approach
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2973,7 +2973,9 @@
       <c r="B146" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C146" s="6"/>
+      <c r="C146" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="4" t="s">

</xml_diff>

<commit_message>
Add NestedInteger interface and NestedIterator class to handle nested lists
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2984,7 +2984,9 @@
       <c r="B147" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C147" s="6"/>
+      <c r="C147" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="4" t="s">

</xml_diff>

<commit_message>
Add TreeNode and InvertBT classes for binary tree operations
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3039,7 +3039,9 @@
       <c r="B154" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C154" s="6"/>
+      <c r="C154" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="4" t="s">
@@ -3048,7 +3050,9 @@
       <c r="B155" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C155" s="6"/>
+      <c r="C155" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="4" t="s">

</xml_diff>

<commit_message>
Add RangeSumBST class to calculate the sum of values within a given range in a binary search tree
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3015,17 +3015,17 @@
       </c>
       <c r="C150" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="17.25">
       <c r="A151" s="4"/>
       <c r="B151" s="7"/>
       <c r="C151" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="17.25">
       <c r="A152" s="4"/>
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="17.25">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
         <v>145</v>
@@ -3061,7 +3061,9 @@
       <c r="B156" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C156" s="6"/>
+      <c r="C156" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="4" t="s">
@@ -3070,7 +3072,9 @@
       <c r="B157" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C157" s="6"/>
+      <c r="C157" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="4" t="s">

</xml_diff>

<commit_message>
Add SymmetricTree class to determine if a binary tree is symmetric around its center
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3083,7 +3083,9 @@
       <c r="B158" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C158" s="6"/>
+      <c r="C158" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="4" t="s">

</xml_diff>

<commit_message>
Add Array2BST class to convert a sorted array into a height-balanced binary search tree
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3015,17 +3015,17 @@
       </c>
       <c r="C150" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="4"/>
       <c r="B151" s="7"/>
       <c r="C151" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="4"/>
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
         <v>145</v>
@@ -3094,7 +3094,9 @@
       <c r="B159" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C159" s="6"/>
+      <c r="C159" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="4" t="s">

</xml_diff>

<commit_message>
Add Merge2BT class to merge two binary trees by summing corresponding nodes
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3105,7 +3105,9 @@
       <c r="B160" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C160" s="6"/>
+      <c r="C160" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="4" t="s">

</xml_diff>

<commit_message>
max depth of bt
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -1572,26 +1572,26 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -3116,7 +3116,9 @@
       <c r="B161" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C161" s="6"/>
+      <c r="C161" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="4" t="s">

</xml_diff>

<commit_message>
Add GetPathsBT class to find all root-to-leaf paths in a binary tree
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2988,7 +2988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
       <c r="A148" s="4" t="s">
         <v>34</v>
       </c>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="C148" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
       <c r="A149" s="4" t="s">
         <v>34</v>
       </c>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="C149" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5">
       <c r="A150" s="4" t="s">
         <v>34</v>
       </c>
@@ -3015,24 +3015,24 @@
       </c>
       <c r="C150" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
       <c r="A151" s="4"/>
       <c r="B151" s="7"/>
       <c r="C151" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5">
       <c r="A152" s="4"/>
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
         <v>145</v>
       </c>
       <c r="C153" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
       <c r="A154" s="4" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
       <c r="A155" s="4" t="s">
         <v>9</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
       <c r="A156" s="4" t="s">
         <v>9</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
       <c r="A157" s="4" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
       <c r="A158" s="4" t="s">
         <v>9</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
       <c r="A159" s="4" t="s">
         <v>9</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
       <c r="A160" s="4" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
       <c r="A161" s="4" t="s">
         <v>9</v>
       </c>
@@ -3120,16 +3120,18 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
       <c r="A162" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C162" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
+      <c r="C162" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
       <c r="A163" s="4" t="s">
         <v>9</v>
       </c>
@@ -3138,7 +3140,7 @@
       </c>
       <c r="C163" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
       <c r="A164" s="4" t="s">
         <v>9</v>
       </c>
@@ -3147,7 +3149,7 @@
       </c>
       <c r="C164" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5">
       <c r="A165" s="4" t="s">
         <v>9</v>
       </c>
@@ -3156,7 +3158,7 @@
       </c>
       <c r="C165" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
       <c r="A166" s="4" t="s">
         <v>9</v>
       </c>
@@ -3165,7 +3167,7 @@
       </c>
       <c r="C166" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5">
       <c r="A167" s="4" t="s">
         <v>9</v>
       </c>
@@ -3174,7 +3176,7 @@
       </c>
       <c r="C167" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5">
       <c r="A168" s="4" t="s">
         <v>9</v>
       </c>
@@ -3183,7 +3185,7 @@
       </c>
       <c r="C168" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
       <c r="A169" s="4" t="s">
         <v>9</v>
       </c>
@@ -3192,7 +3194,7 @@
       </c>
       <c r="C169" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
       <c r="A170" s="4" t="s">
         <v>9</v>
       </c>
@@ -3201,7 +3203,7 @@
       </c>
       <c r="C170" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
       <c r="A171" s="4" t="s">
         <v>9</v>
       </c>
@@ -3210,7 +3212,7 @@
       </c>
       <c r="C171" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
       <c r="A172" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add SameBT class to determine if two binary trees are identical in structure and node values
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3138,7 +3138,9 @@
       <c r="B163" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C163" s="6"/>
+      <c r="C163" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
       <c r="A164" s="4" t="s">

</xml_diff>

<commit_message>
Add LeastCommonAncestorBT class to find the lowest common ancestor of two nodes in a binary search tree
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -2988,7 +2988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="4" t="s">
         <v>34</v>
       </c>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="C148" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="4" t="s">
         <v>34</v>
       </c>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="C149" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="4" t="s">
         <v>34</v>
       </c>
@@ -3015,24 +3015,24 @@
       </c>
       <c r="C150" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="4"/>
       <c r="B151" s="7"/>
       <c r="C151" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="4"/>
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
         <v>145</v>
       </c>
       <c r="C153" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="4" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="4" t="s">
         <v>9</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="4" t="s">
         <v>9</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="4" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="4" t="s">
         <v>9</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="4" t="s">
         <v>9</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="4" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="4" t="s">
         <v>9</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="4" t="s">
         <v>9</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="4" t="s">
         <v>9</v>
       </c>
@@ -3142,14 +3142,16 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C164" s="6"/>
+      <c r="C164" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5">
       <c r="A165" s="4" t="s">

</xml_diff>

<commit_message>
Add PathSumBT class to determine if a path sum equals a target value in a binary tree
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3160,7 +3160,9 @@
       <c r="B165" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C165" s="6"/>
+      <c r="C165" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
       <c r="A166" s="4" t="s">

</xml_diff>

<commit_message>
Add LeftLeavesSumBT class to calculate the sum of left leaves in a binary tree
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3025,14 +3025,14 @@
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
         <v>145</v>
       </c>
       <c r="C153" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
       <c r="A154" s="4" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
       <c r="A155" s="4" t="s">
         <v>9</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
       <c r="A156" s="4" t="s">
         <v>9</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
       <c r="A157" s="4" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
       <c r="A158" s="4" t="s">
         <v>9</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
       <c r="A159" s="4" t="s">
         <v>9</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
       <c r="A160" s="4" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
       <c r="A161" s="4" t="s">
         <v>9</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
       <c r="A162" s="4" t="s">
         <v>9</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
       <c r="A163" s="4" t="s">
         <v>9</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
       <c r="A164" s="4" t="s">
         <v>5</v>
       </c>
@@ -3180,7 +3180,9 @@
       <c r="B167" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C167" s="6"/>
+      <c r="C167" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5">
       <c r="A168" s="4" t="s">
@@ -3227,7 +3229,7 @@
       </c>
       <c r="C172" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
       <c r="A173" s="4" t="s">
         <v>5</v>
       </c>
@@ -3236,7 +3238,7 @@
       </c>
       <c r="C173" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
       <c r="A174" s="4" t="s">
         <v>5</v>
       </c>
@@ -3245,7 +3247,7 @@
       </c>
       <c r="C174" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
       <c r="A175" s="4" t="s">
         <v>5</v>
       </c>
@@ -3254,7 +3256,7 @@
       </c>
       <c r="C175" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5">
       <c r="A176" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add HeightBalancedBT class to check if a binary tree is height-balanced
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3191,7 +3191,9 @@
       <c r="B168" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C168" s="6"/>
+      <c r="C168" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
       <c r="A169" s="4" t="s">

</xml_diff>

<commit_message>
Add InOrderBT class for binary tree inorder traversal
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3211,7 +3211,9 @@
       <c r="B170" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C170" s="6"/>
+      <c r="C170" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
       <c r="A171" s="4" t="s">

</xml_diff>

<commit_message>
Refactor MinAbsDiffBT class to improve minimum difference calculation logic
</commit_message>
<xml_diff>
--- a/DSASheet.xlsx
+++ b/DSASheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="324">
   <si>
     <t>#CrackYourInternship Challenge</t>
   </si>
@@ -3025,14 +3025,14 @@
       <c r="B152" s="7"/>
       <c r="C152" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="4"/>
       <c r="B153" s="14" t="s">
         <v>145</v>
       </c>
       <c r="C153" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="4" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="4" t="s">
         <v>9</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="4" t="s">
         <v>9</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="4" t="s">
         <v>9</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="4" t="s">
         <v>9</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="4" t="s">
         <v>9</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="4" t="s">
         <v>9</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="4" t="s">
         <v>9</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="4" t="s">
         <v>9</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="4" t="s">
         <v>9</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="4" t="s">
         <v>5</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="4" t="s">
         <v>9</v>
       </c>
@@ -3164,16 +3164,18 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C166" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5">
+      <c r="C166" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="4" t="s">
         <v>9</v>
       </c>
@@ -3184,7 +3186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="4" t="s">
         <v>9</v>
       </c>
@@ -3195,7 +3197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="4" t="s">
         <v>9</v>
       </c>
@@ -3204,7 +3206,7 @@
       </c>
       <c r="C169" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="4" t="s">
         <v>9</v>
       </c>
@@ -3215,7 +3217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="4" t="s">
         <v>9</v>
       </c>
@@ -3224,7 +3226,7 @@
       </c>
       <c r="C171" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="4" t="s">
         <v>5</v>
       </c>
@@ -3233,7 +3235,7 @@
       </c>
       <c r="C172" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="4" t="s">
         <v>5</v>
       </c>
@@ -3242,7 +3244,7 @@
       </c>
       <c r="C173" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="4" t="s">
         <v>5</v>
       </c>
@@ -3251,7 +3253,7 @@
       </c>
       <c r="C174" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>